<commit_message>
date changed, insert seconds
</commit_message>
<xml_diff>
--- a/tvData.xlsx
+++ b/tvData.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>05/17/1900</t>
+          <t>05/17/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -487,7 +487,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>05/24/1900</t>
+          <t>05/24/2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>05/27/1900</t>
+          <t>05/27/2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>05/16/1900</t>
+          <t>05/16/2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>05/22/1900</t>
+          <t>05/22/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -595,7 +595,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>05/17/1900</t>
+          <t>05/17/2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>05/26/1900</t>
+          <t>05/26/2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">

</xml_diff>